<commit_message>
latest changes + deliverables
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaspottier/Main/Schoo/IndustryProject/IndustryProject-BeriatricSurgeryG1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8023FE4E-BFEF-7143-BAAB-B24905C9AE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B53A3-5117-BD47-8080-2AD1758FFE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00BCB2CB-A43B-3F46-B7C1-57D73B7C226B}"/>
   </bookViews>
@@ -208,6 +208,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -283,6 +286,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1473,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D851A6-1D1F-9D4A-AA18-ED3D38FCA658}">
   <dimension ref="A4:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="134" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
repair features removed from db, Model, backend  and Frontend
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -2,18 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaspottier/Main/Schoo/IndustryProject/IndustryProject-BeriatricSurgeryG1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B53A3-5117-BD47-8080-2AD1758FFE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E436E5-0717-EC4E-AFB8-927A99F756DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00BCB2CB-A43B-3F46-B7C1-57D73B7C226B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="2" xr2:uid="{00BCB2CB-A43B-3F46-B7C1-57D73B7C226B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -165,7 +167,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Chart</a:t>
+              <a:t> Chart Sprint 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -358,6 +360,880 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EBEB-E94B-9253-03C1C73CE056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1723454448"/>
+        <c:axId val="547052015"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1723454448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547052015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="547052015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1723454448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-058A-5448-BC8D-33F01E130E2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-058A-5448-BC8D-33F01E130E2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1723454448"/>
+        <c:axId val="547052015"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1723454448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547052015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="547052015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1723454448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart Spint 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (3)'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (3)'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-19F2-D140-87EB-7468D5DA10A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (3)'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (3)'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-19F2-D140-87EB-7468D5DA10A0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -603,7 +1479,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1144,6 +3132,92 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400285</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>5457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>6428</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>164729</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C23955FF-3308-E54B-861B-36D814E113EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400285</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>5457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>6428</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>164729</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A538B4C-321A-EA47-82BE-7FC37C9A552C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1477,10 +3551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D851A6-1D1F-9D4A-AA18-ED3D38FCA658}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A4:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView zoomScale="65" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1599,4 +3674,257 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE00A53-8E9B-1C41-9920-9D1551CAA0B2}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A4:F10"/>
+  <sheetViews>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <f>C5</f>
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f>D5/5</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>C5-F6</f>
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <f>D5-$E$5</f>
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>C6-F7</f>
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D10" si="0">D6-$E$5</f>
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f>C7-F8</f>
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>C8-F9</f>
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f>C9-F10</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B741B0F-FC71-4A4E-B6E3-61AE7BB364D3}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A4:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <f>C5</f>
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <f>ROUND(D5/5,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>C5-F6</f>
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <f>D5-$E$5</f>
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>C6-F7</f>
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D10" si="0">D6-$E$5</f>
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C10" si="1">C7-F8</f>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new ai explanation page
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaspottier/Main/Schoo/IndustryProject/IndustryProject-BeriatricSurgeryG1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D82AB92-2467-9D4D-A182-7BBCB38C052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CFB355-7842-9046-A0CE-4652D0706064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="2" xr2:uid="{00BCB2CB-A43B-3F46-B7C1-57D73B7C226B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="3" xr2:uid="{00BCB2CB-A43B-3F46-B7C1-57D73B7C226B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1 (3)" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1 (4)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -1234,6 +1235,443 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-19F2-D140-87EB-7468D5DA10A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1723454448"/>
+        <c:axId val="547052015"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1723454448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547052015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="547052015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1723454448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart Spint 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (4)'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (4)'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DC6-8E4E-8CB8-D27EF2A82E75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (4)'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (4)'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1DC6-8E4E-8CB8-D27EF2A82E75}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1559,6 +1997,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2592,6 +3070,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3212,6 +4206,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A538B4C-321A-EA47-82BE-7FC37C9A552C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400285</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>5457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>6428</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>164729</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1EB2AC-5DD3-7842-ACDA-186515D81981}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3808,7 +4845,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A4:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+    <sheetView zoomScale="143" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -3927,4 +4964,130 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90266803-36F7-0640-9EEC-9D7A01DE608D}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A4:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <f>C5</f>
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <f>ROUND(D5/5,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>C5-F6</f>
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <f>D5-$E$5</f>
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>C6-F7</f>
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D10" si="0">D6-$E$5</f>
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C10" si="1">C7-F8</f>
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>